<commit_message>
End of sprint 1
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord PreTPI.xlsx
+++ b/Documentation/Journal de bord PreTPI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keanu.trosset\Desktop\PréTPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\HotelplanEnMieux\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>120 minutes</t>
+  </si>
+  <si>
+    <t>Revision du sprint 1</t>
   </si>
 </sst>
 </file>
@@ -764,7 +767,7 @@
   <dimension ref="B1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,9 +884,15 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="20"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
+      <c r="C9" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="9">
+        <v>44232</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Template of the website + maquette + MCD-MLD review
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord PreTPI.xlsx
+++ b/Documentation/Journal de bord PreTPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Dossier avec tout reuni + création de la docs</t>
   </si>
   <si>
-    <t>MCD-MLD sur papier</t>
-  </si>
-  <si>
     <t>MCD-MLD au format éléctronique + Correction</t>
   </si>
   <si>
@@ -86,10 +83,31 @@
     <t>45 minutes</t>
   </si>
   <si>
-    <t>120 minutes</t>
-  </si>
-  <si>
     <t>Revision du sprint 1</t>
+  </si>
+  <si>
+    <t>MCD sur papier</t>
+  </si>
+  <si>
+    <t>MLD sur papier</t>
+  </si>
+  <si>
+    <t>20 minutes</t>
+  </si>
+  <si>
+    <t>100 minutes</t>
+  </si>
+  <si>
+    <t>Recherche du templates</t>
+  </si>
+  <si>
+    <t>60 minutes</t>
+  </si>
+  <si>
+    <t>Finition du sprint 1</t>
+  </si>
+  <si>
+    <t>Installation du template</t>
   </si>
 </sst>
 </file>
@@ -486,8 +504,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C2:F80" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="C2:F80"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C2:F81" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="C2:F81"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Tâche" dataDxfId="3"/>
     <tableColumn id="3" name="Date" dataDxfId="2"/>
@@ -764,10 +782,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:F81"/>
+  <dimension ref="B1:F82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,7 +829,7 @@
         <v>44228</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="4"/>
     </row>
@@ -820,37 +838,37 @@
         <v>4</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D4" s="11">
         <v>44228</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F4" s="13"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="9">
+        <v>44228</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D6" s="11">
         <v>44229</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="9">
-        <v>44231</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>16</v>
@@ -859,21 +877,19 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C7" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="9">
         <v>44231</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C8" s="20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D8" s="9">
         <v>44231</v>
@@ -881,42 +897,68 @@
       <c r="E8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C9" s="20" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D9" s="9">
+        <v>44231</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="9">
         <v>44232</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="20"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
+      <c r="E10" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="20"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
+      <c r="C11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="9">
+        <v>44232</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="20"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10"/>
+      <c r="C12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="9">
+        <v>44232</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="20"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
+      <c r="C13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="9">
+        <v>44235</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -1046,7 +1088,7 @@
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="8"/>
+      <c r="C35" s="20"/>
       <c r="D35" s="9"/>
       <c r="E35" s="10"/>
       <c r="F35" s="5"/>
@@ -1315,11 +1357,17 @@
       <c r="E79" s="10"/>
       <c r="F79" s="5"/>
     </row>
-    <row r="81" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C81" s="14"/>
-      <c r="D81" s="15"/>
-      <c r="E81" s="16"/>
-      <c r="F81" s="17"/>
+    <row r="80" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C80" s="8"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="82" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C82" s="14"/>
+      <c r="D82" s="15"/>
+      <c r="E82" s="16"/>
+      <c r="F82" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Journal de bord updated
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord PreTPI.xlsx
+++ b/Documentation/Journal de bord PreTPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -108,6 +108,36 @@
   </si>
   <si>
     <t>Installation du template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installation du logiciel heidiSQL </t>
+  </si>
+  <si>
+    <t>Création de la base de donnée</t>
+  </si>
+  <si>
+    <t>Création et remise en mémoire du MVC</t>
+  </si>
+  <si>
+    <t>Installation du PHP</t>
+  </si>
+  <si>
+    <t>Initialitation du codage php avec le logiciel ATOM</t>
+  </si>
+  <si>
+    <t>Remise en mémoire de l'HTML + modification du template</t>
+  </si>
+  <si>
+    <t>Correction avec un camarade du mld-mcd et maquette</t>
+  </si>
+  <si>
+    <t>50 minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification du template pour qu'il soye a mes attentes + remise en mémoire du codage </t>
+  </si>
+  <si>
+    <t>90 minutes</t>
   </si>
 </sst>
 </file>
@@ -784,8 +814,8 @@
   </sheetPr>
   <dimension ref="B1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,52 +991,100 @@
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="20"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
+    <row r="14" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C14" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="9">
+        <v>44235</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="20"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
+    <row r="15" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="9">
+        <v>44235</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="20"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
+    <row r="16" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C16" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="9">
+        <v>44238</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" s="20"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
+    <row r="17" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C17" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="9">
+        <v>44238</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="20"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
+      <c r="C18" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="9">
+        <v>44238</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="20"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
+      <c r="C19" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="9">
+        <v>44239</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C20" s="20"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10"/>
+      <c r="C20" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="9">
+        <v>44239</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="20"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
+    <row r="21" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C21" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="9">
+        <v>44239</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Last step of the sprint 2
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord PreTPI.xlsx
+++ b/Documentation/Journal de bord PreTPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>Date</t>
   </si>
@@ -138,6 +138,24 @@
   </si>
   <si>
     <t>90 minutes</t>
+  </si>
+  <si>
+    <t>Arborecense du site</t>
+  </si>
+  <si>
+    <t>120 minutes</t>
+  </si>
+  <si>
+    <t>Transcription du template HTML en structure MVC avec redirection</t>
+  </si>
+  <si>
+    <t>Review des points de la docs</t>
+  </si>
+  <si>
+    <t>Regler le bug de mise en page du register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corriger les bugs de la base de donnée </t>
   </si>
 </sst>
 </file>
@@ -814,8 +832,8 @@
   </sheetPr>
   <dimension ref="B1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,33 +1106,63 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="20"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10"/>
+      <c r="C22" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="9">
+        <v>44242</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C23" s="20"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="10"/>
+    <row r="23" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C23" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="9">
+        <v>44245</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C24" s="20"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="10"/>
+      <c r="C24" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="9">
+        <v>44245</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C25" s="20"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="10"/>
+    <row r="25" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C25" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="9">
+        <v>44245</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C26" s="20"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10"/>
+    <row r="26" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C26" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="9">
+        <v>44246</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Login + profil de fini
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord PreTPI.xlsx
+++ b/Documentation/Journal de bord PreTPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -74,15 +74,6 @@
     <t>MCD-MLD au format éléctronique + Correction</t>
   </si>
   <si>
-    <t>30 minutes</t>
-  </si>
-  <si>
-    <t>10 minutes</t>
-  </si>
-  <si>
-    <t>45 minutes</t>
-  </si>
-  <si>
     <t>Revision du sprint 1</t>
   </si>
   <si>
@@ -92,18 +83,9 @@
     <t>MLD sur papier</t>
   </si>
   <si>
-    <t>20 minutes</t>
-  </si>
-  <si>
-    <t>100 minutes</t>
-  </si>
-  <si>
     <t>Recherche du templates</t>
   </si>
   <si>
-    <t>60 minutes</t>
-  </si>
-  <si>
     <t>Finition du sprint 1</t>
   </si>
   <si>
@@ -131,21 +113,12 @@
     <t>Correction avec un camarade du mld-mcd et maquette</t>
   </si>
   <si>
-    <t>50 minutes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Modification du template pour qu'il soye a mes attentes + remise en mémoire du codage </t>
   </si>
   <si>
-    <t>90 minutes</t>
-  </si>
-  <si>
     <t>Arborecense du site</t>
   </si>
   <si>
-    <t>120 minutes</t>
-  </si>
-  <si>
     <t>Transcription du template HTML en structure MVC avec redirection</t>
   </si>
   <si>
@@ -156,6 +129,51 @@
   </si>
   <si>
     <t xml:space="preserve">Corriger les bugs de la base de donnée </t>
+  </si>
+  <si>
+    <t>Probleme de FK</t>
+  </si>
+  <si>
+    <t>Corriger un probleme de MLD</t>
+  </si>
+  <si>
+    <t>Tables intermediaire non relié + fk manquante</t>
+  </si>
+  <si>
+    <t>Cas d'utilisation de la docs a remettre au propre</t>
+  </si>
+  <si>
+    <t>Comprehension de ce qu'on a discuter avec le professeur</t>
+  </si>
+  <si>
+    <t>Creation de la page Creation de voyage</t>
+  </si>
+  <si>
+    <t>Premiere interaction avec la base de donnée</t>
+  </si>
+  <si>
+    <t>Codage du Login</t>
+  </si>
+  <si>
+    <t>Remplissage de la doc</t>
+  </si>
+  <si>
+    <t>Finition du login</t>
+  </si>
+  <si>
+    <t>Bug du login a reparer</t>
+  </si>
+  <si>
+    <t>Gros bug sur la base de donnée et j'ai du changer de manière d'envoyer mes requetes SQL</t>
+  </si>
+  <si>
+    <t>Suite au changement de l'approche de la gestion des requetes certains enorme bug sont aparue</t>
+  </si>
+  <si>
+    <t>Profil</t>
+  </si>
+  <si>
+    <t>Remplisage journal de bord</t>
   </si>
 </sst>
 </file>
@@ -832,8 +850,8 @@
   </sheetPr>
   <dimension ref="B1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,8 +894,8 @@
       <c r="D3" s="6">
         <v>44228</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>16</v>
+      <c r="E3" s="7">
+        <v>45</v>
       </c>
       <c r="F3" s="4"/>
     </row>
@@ -886,25 +904,25 @@
         <v>4</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="11">
         <v>44228</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="12">
         <v>20</v>
       </c>
       <c r="F4" s="13"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C5" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D5" s="9">
         <v>44228</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>21</v>
+      <c r="E5" s="10">
+        <v>100</v>
       </c>
       <c r="F5" s="5"/>
     </row>
@@ -918,8 +936,8 @@
       <c r="D6" s="11">
         <v>44229</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>16</v>
+      <c r="E6" s="10">
+        <v>45</v>
       </c>
       <c r="F6" s="5"/>
     </row>
@@ -930,8 +948,8 @@
       <c r="D7" s="9">
         <v>44231</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>15</v>
+      <c r="E7" s="10">
+        <v>10</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -942,8 +960,8 @@
       <c r="D8" s="9">
         <v>44231</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>15</v>
+      <c r="E8" s="10">
+        <v>10</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>12</v>
@@ -956,267 +974,333 @@
       <c r="D9" s="9">
         <v>44231</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>14</v>
+      <c r="E9" s="10">
+        <v>30</v>
       </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D10" s="9">
         <v>44232</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>14</v>
+      <c r="E10" s="10">
+        <v>30</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C11" s="20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D11" s="9">
         <v>44232</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>14</v>
+      <c r="E11" s="10">
+        <v>30</v>
       </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C12" s="20" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D12" s="9">
         <v>44232</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>23</v>
+      <c r="E12" s="10">
+        <v>60</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C13" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D13" s="9">
         <v>44235</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="10">
         <v>20</v>
       </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C14" s="20" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D14" s="9">
         <v>44235</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="10">
         <v>20</v>
       </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C15" s="20" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D15" s="9">
         <v>44235</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>23</v>
+      <c r="E15" s="10">
+        <v>60</v>
       </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C16" s="20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D16" s="9">
         <v>44238</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="10">
         <v>20</v>
       </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="3:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C17" s="20" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D17" s="9">
         <v>44238</v>
       </c>
-      <c r="E17" s="10" t="s">
-        <v>35</v>
+      <c r="E17" s="10">
+        <v>90</v>
       </c>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="20" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D18" s="9">
         <v>44238</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>14</v>
+      <c r="E18" s="10">
+        <v>30</v>
       </c>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="20" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D19" s="9">
         <v>44239</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>14</v>
+      <c r="E19" s="10">
+        <v>30</v>
       </c>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="20" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D20" s="9">
         <v>44239</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>23</v>
+      <c r="E20" s="10">
+        <v>60</v>
       </c>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C21" s="20" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D21" s="9">
         <v>44239</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>33</v>
+      <c r="E21" s="10">
+        <v>50</v>
       </c>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" s="20" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D22" s="9">
         <v>44242</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>37</v>
+      <c r="E22" s="10">
+        <v>120</v>
       </c>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C23" s="20" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D23" s="9">
         <v>44245</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>37</v>
+      <c r="E23" s="10">
+        <v>120</v>
       </c>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C24" s="20" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D24" s="9">
         <v>44245</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="10">
         <v>20</v>
       </c>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C25" s="20" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D25" s="9">
         <v>44245</v>
       </c>
-      <c r="E25" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="5"/>
+      <c r="E25" s="10">
+        <v>60</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="26" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C26" s="20" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D26" s="9">
         <v>44246</v>
       </c>
-      <c r="E26" s="10" t="s">
-        <v>23</v>
+      <c r="E26" s="10">
+        <v>60</v>
       </c>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C27" s="20"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C28" s="20"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C29" s="20"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="10"/>
+      <c r="C27" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="9">
+        <v>44256</v>
+      </c>
+      <c r="E27" s="10">
+        <v>20</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C28" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="9">
+        <v>44256</v>
+      </c>
+      <c r="E28" s="10">
+        <v>30</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C29" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="9">
+        <v>44256</v>
+      </c>
+      <c r="E29" s="10">
+        <v>120</v>
+      </c>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C30" s="20"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="5"/>
+    <row r="30" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C30" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="9">
+        <v>44259</v>
+      </c>
+      <c r="E30" s="10">
+        <v>120</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C31" s="20"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="10"/>
+      <c r="C31" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="9">
+        <v>44259</v>
+      </c>
+      <c r="E31" s="10">
+        <v>120</v>
+      </c>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="20"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="5"/>
+    <row r="32" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C32" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="9">
+        <v>44259</v>
+      </c>
+      <c r="E32" s="10">
+        <v>120</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="20"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="5"/>
+      <c r="C33" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="9">
+        <v>44260</v>
+      </c>
+      <c r="E33" s="10">
+        <v>120</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="20"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="10"/>
+      <c r="C34" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="9">
+        <v>44260</v>
+      </c>
+      <c r="E34" s="10">
+        <v>40</v>
+      </c>
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="20"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="10"/>
+      <c r="C35" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="9">
+        <v>44260</v>
+      </c>
+      <c r="E35" s="10">
+        <v>20</v>
+      </c>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Journal de bord PreTPI.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord PreTPI.xlsx
+++ b/Documentation/Journal de bord PreTPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -180,6 +180,36 @@
   </si>
   <si>
     <t>CRUD</t>
+  </si>
+  <si>
+    <t>Rattrapage du retard</t>
+  </si>
+  <si>
+    <t>Affichage des travels sur le menu home</t>
+  </si>
+  <si>
+    <t>Affichage des travels sur le profil</t>
+  </si>
+  <si>
+    <t>Update du mail + password sur profil</t>
+  </si>
+  <si>
+    <t>Bug d'envoie de fichier trop grand</t>
+  </si>
+  <si>
+    <t>PHP.INI bugait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bug sur l'affichage des travels sur home </t>
+  </si>
+  <si>
+    <t>La taille des div était variables donc c'était pas beau</t>
+  </si>
+  <si>
+    <t>probleme d'affichage des erreurs</t>
+  </si>
+  <si>
+    <t>Quand on se trompait de psw ou email</t>
   </si>
 </sst>
 </file>
@@ -865,8 +895,8 @@
   </sheetPr>
   <dimension ref="B1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="E24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,41 +1362,85 @@
       </c>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C37" s="20"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="5"/>
+    <row r="37" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C37" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="21">
+        <v>44263</v>
+      </c>
+      <c r="E37" s="22">
+        <v>120</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C38" s="20"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="22"/>
+      <c r="C38" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="21">
+        <v>44266</v>
+      </c>
+      <c r="E38" s="22">
+        <v>60</v>
+      </c>
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C39" s="20"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="22"/>
+      <c r="C39" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="21">
+        <v>44266</v>
+      </c>
+      <c r="E39" s="22">
+        <v>120</v>
+      </c>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C40" s="20"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="5"/>
+      <c r="C40" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" s="9">
+        <v>44266</v>
+      </c>
+      <c r="E40" s="10">
+        <v>60</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C41" s="20"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C42" s="20"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="5"/>
+      <c r="C41" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="9">
+        <v>44267</v>
+      </c>
+      <c r="E41" s="10">
+        <v>60</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C42" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" s="21">
+        <v>44267</v>
+      </c>
+      <c r="E42" s="22">
+        <v>120</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C43" s="20"/>

</xml_diff>

<commit_message>
changement on the profil and createtravel
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord PreTPI.xlsx
+++ b/Documentation/Journal de bord PreTPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>Quand on se trompait de psw ou email</t>
+  </si>
+  <si>
+    <t>Mise en ligne du site sur Swisscenter</t>
   </si>
 </sst>
 </file>
@@ -895,8 +898,8 @@
   </sheetPr>
   <dimension ref="B1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="C24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,9 +1464,15 @@
       <c r="F45" s="5"/>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C46" s="20"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="22"/>
+      <c r="C46" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="21">
+        <v>44273</v>
+      </c>
+      <c r="E46" s="22">
+        <v>60</v>
+      </c>
       <c r="F46" s="5"/>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
last modification + documentation
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord PreTPI.xlsx
+++ b/Documentation/Journal de bord PreTPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>Date</t>
   </si>
@@ -213,6 +213,72 @@
   </si>
   <si>
     <t>Mise en ligne du site sur Swisscenter</t>
+  </si>
+  <si>
+    <t>Mise en ligne de la base de donnée sur Swisscenter</t>
+  </si>
+  <si>
+    <t>D'abords tester en FTP puis remarquer que il y a une console de gestion phpmyadmin.</t>
+  </si>
+  <si>
+    <t>Remplissage de la documentation + quelque commentaire sur le code</t>
+  </si>
+  <si>
+    <t>Creation de l'historique de voyage</t>
+  </si>
+  <si>
+    <t>Codage de la page, inserstion SQL etc.</t>
+  </si>
+  <si>
+    <t>Reglage d'un bug interface sur l'historique</t>
+  </si>
+  <si>
+    <t>Rajout du nombre de chose que l'on veut prendre dans la checklist</t>
+  </si>
+  <si>
+    <t>Reglage d'un bug a la creation d'un voyage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les filtres ne s'affichaient pas correctement </t>
+  </si>
+  <si>
+    <t>Avec le champ si s'affiche ou non si la case est coché</t>
+  </si>
+  <si>
+    <t>Plusieurs soucis venait quand je creait un voyage d'on je n'avais pas remarquer l'existance jusqu’à present</t>
+  </si>
+  <si>
+    <t>Reglage de quelque bug sur le Swisscenter</t>
+  </si>
+  <si>
+    <t>Certaines pages ne s'affichait pas comme en local.</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Creation du manuel utilisateur</t>
+  </si>
+  <si>
+    <t>Introduction a l'export PDF</t>
+  </si>
+  <si>
+    <t>Recherche d'une librairie, apprentissage de commence fonctionne une librairie et comment fonctionne cette librairie. Essai et echec.</t>
+  </si>
+  <si>
+    <t>Export PDF</t>
+  </si>
+  <si>
+    <t>Bug de CSS, puis nom transfer de l'image, puis pleins d'autre probleme au fur et a mesure que je continuais.</t>
+  </si>
+  <si>
+    <t>Modifier une annonce</t>
+  </si>
+  <si>
+    <t>Bug sur la modification d'une annonce</t>
+  </si>
+  <si>
+    <t>Probleme avec les checklist</t>
   </si>
 </sst>
 </file>
@@ -898,8 +964,8 @@
   </sheetPr>
   <dimension ref="B1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="C28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,94 +1512,190 @@
       </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="20"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="22"/>
+      <c r="C43" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="21">
+        <v>44270</v>
+      </c>
+      <c r="E43" s="22">
+        <v>120</v>
+      </c>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C44" s="20"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="5"/>
+    <row r="44" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C44" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="21">
+        <v>44270</v>
+      </c>
+      <c r="E44" s="22">
+        <v>60</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="20"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="22"/>
+      <c r="C45" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="21">
+        <v>44273</v>
+      </c>
+      <c r="E45" s="22">
+        <v>60</v>
+      </c>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C46" s="20" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D46" s="21">
         <v>44273</v>
       </c>
-      <c r="E46" s="22">
+      <c r="E46" s="10">
         <v>60</v>
       </c>
       <c r="F46" s="5"/>
     </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C47" s="20"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="5"/>
+    <row r="47" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C47" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="21">
+        <v>44274</v>
+      </c>
+      <c r="E47" s="22">
+        <v>150</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C48" s="20"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="5"/>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C49" s="20"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="5"/>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C50" s="20"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="5"/>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C51" s="20"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="5"/>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C52" s="20"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="5"/>
+      <c r="C48" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="21">
+        <v>44277</v>
+      </c>
+      <c r="E48" s="22">
+        <v>120</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C49" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D49" s="21">
+        <v>44277</v>
+      </c>
+      <c r="E49" s="22">
+        <v>60</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C50" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D50" s="21">
+        <v>44280</v>
+      </c>
+      <c r="E50" s="22">
+        <v>120</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C51" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D51" s="21">
+        <v>44280</v>
+      </c>
+      <c r="E51" s="22">
+        <v>60</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C52" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D52" s="21">
+        <v>44280</v>
+      </c>
+      <c r="E52" s="22">
+        <v>120</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C53" s="20"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="22"/>
+      <c r="C53" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D53" s="21">
+        <v>44280</v>
+      </c>
+      <c r="E53" s="22">
+        <v>60</v>
+      </c>
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C54" s="20"/>
-      <c r="D54" s="21"/>
-      <c r="E54" s="22"/>
+      <c r="C54" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D54" s="21">
+        <v>44280</v>
+      </c>
+      <c r="E54" s="22">
+        <v>60</v>
+      </c>
       <c r="F54" s="5"/>
     </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C55" s="20"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="5"/>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C56" s="20"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="5"/>
+    <row r="55" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C55" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="21">
+        <v>44281</v>
+      </c>
+      <c r="E55" s="22">
+        <v>180</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C56" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D56" s="21">
+        <v>44284</v>
+      </c>
+      <c r="E56" s="22">
+        <v>120</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C57" s="20"/>

</xml_diff>